<commit_message>
Added inquiries in SIQ
Signed-off-by: mariam-elshakafi <mariam.elshakafi@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/PO3_DGW_SIQ.xlsx
+++ b/Input Documents/PO3_DGW_SIQ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iTi_Workspace\SE_Workspace\SWENG_PO3_DigitalWatch\Input Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDC69F5-F65F-43C4-BFED-4E83A0DE3952}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4B4948-C4B5-41AD-9A88-8BE8BBD13B29}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
   <si>
     <t>Status</t>
   </si>
@@ -239,12 +239,126 @@
 The stop watch will be like this 00:00:00
 When you leave the stop watch just reset it </t>
   </si>
+  <si>
+    <t>PO3_DGW_SIQ_08</t>
+  </si>
+  <si>
+    <t>Change mode, don't save adjustments</t>
+  </si>
+  <si>
+    <t>21/2/2020</t>
+  </si>
+  <si>
+    <t>If MODE button is pressed during time adjust or alarm adjust, does it:
+1. Change mode without saving.
+2. Change mode with saving.
+3. Stay in the same mode without saving (Cancel). 
+4. Stay in the same mode without saving?</t>
+  </si>
+  <si>
+    <t>What is displayed on LCD in Alarm mode?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current time, until alarm time is reached </t>
+  </si>
+  <si>
+    <t>If Alarm time is adjusted, and mode is changed to display time or stopwatch, does it still trigger buzzer if alarm time is reached?</t>
+  </si>
+  <si>
+    <t>PO3_DGW_SIQ_09</t>
+  </si>
+  <si>
+    <t>PO3_DGW_SIQ_10</t>
+  </si>
+  <si>
+    <t>If alarm is working in all modes, How can we set alarm to infinity? (Never trigger a buzzer)</t>
+  </si>
+  <si>
+    <t>PO3_DGW_SIQ_11</t>
+  </si>
+  <si>
+    <t>PO3_DGW_SIQ_12</t>
+  </si>
+  <si>
+    <t>What are the initial states for current time, alarm time?</t>
+  </si>
+  <si>
+    <t>Set to a time that's not valid (e.g: 00:00:00)</t>
+  </si>
+  <si>
+    <t>Current time: 12:00:00 AM
+Alarm time: infinity (e.g: 00:00:00)</t>
+  </si>
+  <si>
+    <t>What are the limits for incrementing in adjust mode (for both: current time and alarm)? What happens if we increment to a boundary value?</t>
+  </si>
+  <si>
+    <t>PO3_DGW_SIQ_13</t>
+  </si>
+  <si>
+    <t>PO3_DGW_CRS_F_02</t>
+  </si>
+  <si>
+    <t>PO3_DGW_CRS_F_01
+PO3_DGW_CRS_F_02</t>
+  </si>
+  <si>
+    <t>PO3_DGW_CRS_KE_03</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Current time:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Hours -&gt; 1:12 (reset to 1)
+Minutes -&gt; 0:59 (reset to 0)
+keep AM/PM as they were if hours are incremented above boundary value.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alarm: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Same, but add an option for infinity</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +409,12 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -954,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1242,12 +1362,156 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:12" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:12" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:12" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:12" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:12" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="1" customFormat="1" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="1" customFormat="1" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="1" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="17" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1275,6 +1539,7 @@
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A1:I1"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="H4:H86">
     <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="Problems">
       <formula>NOT(ISERROR(SEARCH("Problems",H4)))</formula>

</xml_diff>

<commit_message>
SIQ Signed-off-by: AmrElnobe <ibrahimamr222@hotmial.com>
</commit_message>
<xml_diff>
--- a/Input Documents/PO3_DGW_SIQ.xlsx
+++ b/Input Documents/PO3_DGW_SIQ.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iTi_Workspace\SE_Workspace\SWENG_PO3_DigitalWatch\Input Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amr Ibrahim\Documents\hola\Input Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4B4948-C4B5-41AD-9A88-8BE8BBD13B29}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="SIQ" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="75">
   <si>
     <t>Status</t>
   </si>
@@ -353,11 +352,23 @@
       <t>Same, but add an option for infinity</t>
     </r>
   </si>
+  <si>
+    <t>PO3_DGW_SIQ_14</t>
+  </si>
+  <si>
+    <t>Amr</t>
+  </si>
+  <si>
+    <t>22/2/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What to do when alarm is reached when mode is in another mode </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -758,18 +769,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:I38" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A3:I38" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:I38" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A3:I38"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Requirement ID" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Asked by" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="SIQ ID" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Question" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Proposed Answer" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Proposed by" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Status" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Answer" dataDxfId="0"/>
+    <tableColumn id="1" name="Requirement ID" dataDxfId="8"/>
+    <tableColumn id="2" name="Asked by" dataDxfId="7"/>
+    <tableColumn id="3" name="SIQ ID" dataDxfId="6"/>
+    <tableColumn id="4" name="Question" dataDxfId="5"/>
+    <tableColumn id="5" name="Proposed Answer" dataDxfId="4"/>
+    <tableColumn id="11" name="Proposed by" dataDxfId="3"/>
+    <tableColumn id="6" name="Date" dataDxfId="2"/>
+    <tableColumn id="7" name="Status" dataDxfId="1"/>
+    <tableColumn id="8" name="Answer" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1071,27 +1082,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="25.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="40.77734375" style="3" customWidth="1"/>
-    <col min="5" max="6" width="30.77734375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="25.77734375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="20.77734375" style="3" customWidth="1"/>
+    <col min="1" max="3" width="25.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="3" customWidth="1"/>
+    <col min="5" max="6" width="30.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="3" customWidth="1"/>
     <col min="9" max="9" width="53" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.77734375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="3" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="3"/>
+    <col min="10" max="10" width="6.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -1104,7 +1115,7 @@
       <c r="H1" s="12"/>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1128,7 @@
       <c r="H2" s="9"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="4" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1150,7 +1161,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1184,7 +1195,7 @@
       </c>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -1218,7 +1229,7 @@
       </c>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1249,7 +1260,7 @@
       <c r="J6" s="5"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -1275,7 +1286,7 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1301,7 +1312,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -1333,7 +1344,7 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -1362,7 +1373,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1388,7 +1399,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" s="1" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
@@ -1414,7 +1425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" s="1" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>67</v>
       </c>
@@ -1434,7 +1445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>67</v>
       </c>
@@ -1460,7 +1471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
@@ -1486,7 +1497,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" s="1" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -1512,28 +1523,47 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:I2"/>
@@ -1552,7 +1582,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Status Error" error="Choose from the drop-down list" sqref="H4:H38" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Status Error" error="Choose from the drop-down list" sqref="H4:H38">
       <formula1>$K$3:$K$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added another question to SIQ
Signed-off-by: mariam-elshakafi <mariam.elshakafi@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/PO3_DGW_SIQ.xlsx
+++ b/Input Documents/PO3_DGW_SIQ.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amr Ibrahim\Documents\hola\Input Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iTi_Workspace\SE_Workspace\SWENG_PO3_DigitalWatch\Input Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005925BB-5A4D-45D1-A3CB-9D64EF7F2C87}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIQ" sheetId="1" r:id="rId1"/>
@@ -261,9 +262,6 @@
     <t xml:space="preserve">Current time, until alarm time is reached </t>
   </si>
   <si>
-    <t>If Alarm time is adjusted, and mode is changed to display time or stopwatch, does it still trigger buzzer if alarm time is reached?</t>
-  </si>
-  <si>
     <t>PO3_DGW_SIQ_09</t>
   </si>
   <si>
@@ -362,13 +360,16 @@
     <t>22/2/2020</t>
   </si>
   <si>
-    <t xml:space="preserve">What to do when alarm is reached when mode is in another mode </t>
+    <t>What to do when alarm is reached if mode is in another mode?</t>
+  </si>
+  <si>
+    <t>If user doesn't stop alarm manually, for how long does it keep ringing?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -572,164 +573,6 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -750,6 +593,164 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -769,18 +770,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:I38" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A3:I38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:I37" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A3:I37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Requirement ID" dataDxfId="8"/>
-    <tableColumn id="2" name="Asked by" dataDxfId="7"/>
-    <tableColumn id="3" name="SIQ ID" dataDxfId="6"/>
-    <tableColumn id="4" name="Question" dataDxfId="5"/>
-    <tableColumn id="5" name="Proposed Answer" dataDxfId="4"/>
-    <tableColumn id="11" name="Proposed by" dataDxfId="3"/>
-    <tableColumn id="6" name="Date" dataDxfId="2"/>
-    <tableColumn id="7" name="Status" dataDxfId="1"/>
-    <tableColumn id="8" name="Answer" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Requirement ID" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Asked by" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="SIQ ID" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Question" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Proposed Answer" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Proposed by" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Status" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Answer" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1082,27 +1083,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="25.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" style="3" customWidth="1"/>
-    <col min="5" max="6" width="30.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="3" customWidth="1"/>
+    <col min="1" max="3" width="25.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="30.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="3" customWidth="1"/>
     <col min="9" max="9" width="53" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="3" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="3"/>
+    <col min="10" max="10" width="6.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="3" hidden="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -1115,7 +1116,7 @@
       <c r="H1" s="12"/>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1128,7 +1129,7 @@
       <c r="H2" s="9"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="4" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1161,7 +1162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1195,7 +1196,7 @@
       </c>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -1229,7 +1230,7 @@
       </c>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1260,7 +1261,7 @@
       <c r="J6" s="5"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -1286,7 +1287,7 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1312,7 +1313,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -1344,7 +1345,7 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -1373,7 +1374,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1399,15 +1400,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="1" customFormat="1" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>54</v>
@@ -1425,41 +1426,41 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>18</v>
@@ -1471,21 +1472,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>18</v>
@@ -1497,21 +1498,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="1" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>18</v>
@@ -1523,66 +1524,65 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B17" s="1" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:8" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:8" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" s="1" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="H4:H86">
-    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="Problems">
+  <conditionalFormatting sqref="H4:H85">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Problems">
       <formula>NOT(ISERROR(SEARCH("Problems",H4)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="12" priority="2" operator="beginsWith" text="Answered">
+    <cfRule type="beginsWith" dxfId="1" priority="2" operator="beginsWith" text="Answered">
       <formula>LEFT(H4,LEN("Answered"))="Answered"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="11" priority="3" operator="beginsWith" text="Not">
+    <cfRule type="beginsWith" dxfId="0" priority="3" operator="beginsWith" text="Not">
       <formula>LEFT(H4,LEN("Not"))="Not"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Status Error" error="Choose from the drop-down list" sqref="H4:H38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Status Error" error="Choose from the drop-down list" sqref="H4:H37" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$K$3:$K$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Modified CYRS to cover review points (9 to 16) IN SIQ
Signed-off-by: AmrElnobe <ibrahimamr222@hotmial.com>
</commit_message>
<xml_diff>
--- a/Input Documents/PO3_DGW_SIQ.xlsx
+++ b/Input Documents/PO3_DGW_SIQ.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TIMS\Documents\GitHub\DGW_Mariam\Input Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amr Ibrahim\Music\HOLA28\Input Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="82">
   <si>
     <t>Status</t>
   </si>
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E15" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="E14" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1417,7 +1417,7 @@
         <v>52</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>75</v>
@@ -1446,7 +1446,7 @@
         <v>52</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>76</v>
@@ -1469,7 +1469,7 @@
         <v>72</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>77</v>
@@ -1498,7 +1498,7 @@
         <v>52</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>78</v>
@@ -1527,7 +1527,7 @@
         <v>52</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>79</v>
@@ -1556,7 +1556,7 @@
         <v>52</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>80</v>
@@ -1579,7 +1579,7 @@
         <v>72</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>81</v>

</xml_diff>